<commit_message>
updated the codesystems and valuesets
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-AdministerVaccine.xlsx
+++ b/output/StructureDefinition-AdministerVaccine.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-25T06:29:04+01:00</t>
+    <t>2025-06-25T15:41:07+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -746,40 +746,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="37.1484375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="37.1484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.79296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="7.046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.265625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.6875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="10.51171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="39.0234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="39.0234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.890625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.29296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.21484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.55078125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.1171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.75390625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="14.375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="15.1015625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="12.26171875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="12.4765625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="7.80078125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="13.609375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="13.91796875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="15.01171875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="7.93359375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.08984375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="14.4296875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.31640625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="17.08203125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="15.18359375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="21.1328125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.98046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="16.2578125" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.54296875" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="11.3203125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="37.1484375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="8.22265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="8.53125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="16.9609375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="15.3125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.33984375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.6953125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="15.98046875" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.44140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="39.0234375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.51953125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="8.859375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
   </cols>
   <sheetData>

</xml_diff>